<commit_message>
1) ADicioniadas 3 disciplinas do PIPGEs
</commit_message>
<xml_diff>
--- a/Elenco SME_2025-2-ICMC_corrigido.xlsx
+++ b/Elenco SME_2025-2-ICMC_corrigido.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="222">
   <si>
     <t xml:space="preserve">Elenco de disciplinas SME para 2025-2</t>
   </si>
@@ -615,27 +615,6 @@
     <t xml:space="preserve">Sistemas Complexos</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">PPG-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">CCMC</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">SME5962</t>
   </si>
   <si>
@@ -726,6 +705,9 @@
     <t xml:space="preserve">Tópicos de pesquisa II </t>
   </si>
   <si>
+    <t xml:space="preserve">EST5108</t>
+  </si>
+  <si>
     <t xml:space="preserve">EST5519</t>
   </si>
   <si>
@@ -742,6 +724,18 @@
   </si>
   <si>
     <t xml:space="preserve">Tópicos Avançados de Pesquisa I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EST5523</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confiabilidade e Análise de Sobrevivência</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EST5527</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modelos de Séries Temporais</t>
   </si>
   <si>
     <t xml:space="preserve">EST5822</t>
@@ -757,7 +751,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -839,12 +833,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -920,7 +908,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -989,26 +977,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1083,10 +1051,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1168,16 +1132,16 @@
   </sheetPr>
   <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F55" activeCellId="0" sqref="F55"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B77" activeCellId="0" sqref="B77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.85"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="25.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="1" width="20.42"/>
@@ -1186,7 +1150,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="19.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="36"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="15" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="15" style="1" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1813,17 +1777,17 @@
       <c r="M21" s="11"/>
       <c r="N21" s="11"/>
     </row>
-    <row r="22" s="21" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="17" t="s">
+    <row r="22" s="15" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="19" t="n">
+      <c r="D22" s="12" t="n">
         <v>1</v>
       </c>
       <c r="E22" s="11" t="s">
@@ -1832,28 +1796,28 @@
       <c r="F22" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="J22" s="20"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17"/>
-    </row>
-    <row r="23" s="21" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="17" t="s">
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J22" s="13"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+    </row>
+    <row r="23" s="15" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="19" t="n">
+      <c r="D23" s="12" t="n">
         <v>1</v>
       </c>
       <c r="E23" s="11" t="s">
@@ -1862,761 +1826,761 @@
       <c r="F23" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="J23" s="20"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="17"/>
-    </row>
-    <row r="24" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="22" t="s">
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J23" s="13"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+    </row>
+    <row r="24" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="E24" s="22" t="s">
+      <c r="D24" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22" t="s">
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="J24" s="22"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="17"/>
-      <c r="N24" s="17"/>
-    </row>
-    <row r="25" s="21" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="22" t="s">
+      <c r="J24" s="17"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+    </row>
+    <row r="25" s="15" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="E25" s="22" t="s">
+      <c r="D25" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17" t="s">
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="J25" s="20"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="17"/>
-    </row>
-    <row r="26" s="21" customFormat="true" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="22" t="s">
+      <c r="J25" s="13"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+    </row>
+    <row r="26" s="15" customFormat="true" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="D26" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="E26" s="22" t="s">
+      <c r="D26" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17" t="s">
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="J26" s="20"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17"/>
-    </row>
-    <row r="27" s="21" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="25" t="s">
+      <c r="J26" s="13"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+    </row>
+    <row r="27" s="15" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="D27" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="E27" s="25" t="s">
+      <c r="D27" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="F27" s="25" t="s">
+      <c r="F27" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="17"/>
-    </row>
-    <row r="28" s="21" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="20" t="s">
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="11"/>
+    </row>
+    <row r="28" s="15" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D28" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="E28" s="17" t="s">
+      <c r="D28" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E28" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="F28" s="17" t="s">
+      <c r="F28" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="J28" s="20"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="17"/>
-    </row>
-    <row r="29" s="21" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="20" t="s">
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J28" s="13"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+    </row>
+    <row r="29" s="15" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D29" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="E29" s="17" t="s">
+      <c r="D29" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="E29" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="F29" s="17" t="s">
+      <c r="F29" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="J29" s="20"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
-      <c r="M29" s="17"/>
-      <c r="N29" s="17"/>
-    </row>
-    <row r="30" s="21" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="20" t="s">
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J29" s="13"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+    </row>
+    <row r="30" s="15" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D30" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="E30" s="17" t="s">
+      <c r="D30" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E30" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="J30" s="20"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="17"/>
-      <c r="N30" s="17"/>
-    </row>
-    <row r="31" s="31" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="30" t="s">
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J30" s="13"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+    </row>
+    <row r="31" s="26" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="D31" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="E31" s="20" t="s">
+      <c r="D31" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="F31" s="20" t="s">
+      <c r="F31" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="20"/>
-    </row>
-    <row r="32" s="31" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="20" t="s">
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+    </row>
+    <row r="32" s="26" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C32" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="D32" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="E32" s="20" t="s">
+      <c r="D32" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="F32" s="20" t="s">
+      <c r="F32" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="20"/>
-      <c r="M32" s="20"/>
-      <c r="N32" s="20"/>
-    </row>
-    <row r="33" s="31" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="20" t="s">
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+    </row>
+    <row r="33" s="26" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="B33" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="D33" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="E33" s="20" t="s">
+      <c r="D33" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="E33" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="F33" s="20" t="s">
+      <c r="F33" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="20"/>
-      <c r="M33" s="20"/>
-      <c r="N33" s="20"/>
-    </row>
-    <row r="34" s="31" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="20" t="s">
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+    </row>
+    <row r="34" s="26" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="C34" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="D34" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="E34" s="20" t="s">
+      <c r="D34" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="F34" s="20" t="s">
+      <c r="F34" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="20"/>
-      <c r="M34" s="20"/>
-      <c r="N34" s="20"/>
-    </row>
-    <row r="35" s="31" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="32" t="s">
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
+    </row>
+    <row r="35" s="26" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B35" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="D35" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="E35" s="20" t="s">
+      <c r="D35" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="E35" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="F35" s="20" t="s">
+      <c r="F35" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-      <c r="I35" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="J35" s="20"/>
-      <c r="K35" s="20"/>
-      <c r="L35" s="20"/>
-      <c r="M35" s="20"/>
-      <c r="N35" s="20"/>
-    </row>
-    <row r="36" s="31" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="20" t="s">
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+    </row>
+    <row r="36" s="26" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C36" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="D36" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="E36" s="20" t="s">
+      <c r="D36" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="F36" s="20" t="s">
+      <c r="F36" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
-      <c r="I36" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
-      <c r="L36" s="20"/>
-      <c r="M36" s="20"/>
-      <c r="N36" s="20"/>
-    </row>
-    <row r="37" s="34" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="22" t="s">
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+    </row>
+    <row r="37" s="29" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="C37" s="22" t="s">
+      <c r="C37" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="D37" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="E37" s="22" t="s">
+      <c r="D37" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="J37" s="23"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="22"/>
-      <c r="M37" s="22"/>
-      <c r="N37" s="22"/>
-    </row>
-    <row r="38" s="34" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="22" t="s">
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J37" s="18"/>
+      <c r="K37" s="17"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="17"/>
+      <c r="N37" s="17"/>
+    </row>
+    <row r="38" s="29" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="C38" s="22" t="s">
+      <c r="C38" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="D38" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="E38" s="22" t="s">
+      <c r="D38" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="22" t="s">
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="J38" s="22"/>
-      <c r="K38" s="22"/>
-      <c r="L38" s="22"/>
-      <c r="M38" s="22"/>
-      <c r="N38" s="22"/>
-    </row>
-    <row r="39" s="34" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="22" t="s">
+      <c r="J38" s="17"/>
+      <c r="K38" s="17"/>
+      <c r="L38" s="17"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="17"/>
+    </row>
+    <row r="39" s="29" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="C39" s="22" t="s">
+      <c r="C39" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="D39" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="E39" s="22" t="s">
+      <c r="D39" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="22" t="s">
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="J39" s="22"/>
-      <c r="K39" s="22"/>
-      <c r="L39" s="22"/>
-      <c r="M39" s="22"/>
-      <c r="N39" s="22"/>
-    </row>
-    <row r="40" s="34" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="22" t="s">
+      <c r="J39" s="17"/>
+      <c r="K39" s="17"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="17"/>
+    </row>
+    <row r="40" s="29" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="C40" s="22" t="s">
+      <c r="C40" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="D40" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="E40" s="22" t="s">
+      <c r="D40" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="E40" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="J40" s="22"/>
-      <c r="K40" s="22"/>
-      <c r="L40" s="22"/>
-      <c r="M40" s="22"/>
-      <c r="N40" s="22"/>
-    </row>
-    <row r="41" s="34" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="22" t="s">
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J40" s="17"/>
+      <c r="K40" s="17"/>
+      <c r="L40" s="17"/>
+      <c r="M40" s="17"/>
+      <c r="N40" s="17"/>
+    </row>
+    <row r="41" s="29" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="B41" s="22" t="s">
+      <c r="B41" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="C41" s="22" t="s">
+      <c r="C41" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="D41" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="E41" s="22" t="s">
+      <c r="D41" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="F41" s="22"/>
-      <c r="G41" s="22"/>
-      <c r="H41" s="22"/>
-      <c r="I41" s="22" t="s">
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="J41" s="22"/>
-      <c r="K41" s="22"/>
-      <c r="L41" s="22"/>
-      <c r="M41" s="22"/>
-      <c r="N41" s="22"/>
-    </row>
-    <row r="42" s="21" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="35" t="s">
+      <c r="J41" s="17"/>
+      <c r="K41" s="17"/>
+      <c r="L41" s="17"/>
+      <c r="M41" s="17"/>
+      <c r="N41" s="17"/>
+    </row>
+    <row r="42" s="15" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="B42" s="35" t="s">
+      <c r="B42" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="C42" s="35" t="s">
+      <c r="C42" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="D42" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="E42" s="37" t="s">
+      <c r="D42" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="E42" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="F42" s="37" t="s">
+      <c r="F42" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17"/>
-      <c r="I42" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="J42" s="17"/>
-      <c r="K42" s="17"/>
-      <c r="L42" s="17"/>
-      <c r="M42" s="17"/>
-      <c r="N42" s="17"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J42" s="11"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
+      <c r="N42" s="11"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="35" t="s">
+      <c r="A43" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="B43" s="35" t="s">
+      <c r="B43" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="C43" s="35" t="s">
+      <c r="C43" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="D43" s="36" t="n">
+      <c r="D43" s="31" t="n">
         <v>2</v>
       </c>
-      <c r="E43" s="38" t="s">
+      <c r="E43" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="F43" s="38" t="s">
+      <c r="F43" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
       <c r="I43" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="35" t="s">
+      <c r="A44" s="30" t="s">
         <v>149</v>
       </c>
-      <c r="B44" s="35" t="s">
+      <c r="B44" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="C44" s="37" t="s">
+      <c r="C44" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="D44" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="E44" s="37" t="s">
+      <c r="D44" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="E44" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="F44" s="37" t="s">
+      <c r="F44" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="G44" s="17"/>
-      <c r="H44" s="17"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
       <c r="I44" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="30" t="s">
         <v>149</v>
       </c>
-      <c r="B45" s="35" t="s">
+      <c r="B45" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="C45" s="35" t="s">
+      <c r="C45" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="D45" s="36" t="n">
+      <c r="D45" s="31" t="n">
         <v>2</v>
       </c>
-      <c r="E45" s="38" t="s">
+      <c r="E45" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="F45" s="38" t="s">
+      <c r="F45" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
       <c r="I45" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="35" t="s">
+      <c r="A46" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="B46" s="35" t="s">
+      <c r="B46" s="30" t="s">
         <v>156</v>
       </c>
-      <c r="C46" s="35" t="s">
+      <c r="C46" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="D46" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="E46" s="37" t="s">
+      <c r="D46" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="E46" s="32" t="s">
         <v>158</v>
       </c>
-      <c r="F46" s="37" t="s">
+      <c r="F46" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
       <c r="I46" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="35" t="s">
+      <c r="A47" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="B47" s="35" t="s">
+      <c r="B47" s="30" t="s">
         <v>156</v>
       </c>
-      <c r="C47" s="35" t="s">
+      <c r="C47" s="30" t="s">
         <v>159</v>
       </c>
-      <c r="D47" s="39" t="n">
+      <c r="D47" s="34" t="n">
         <v>2</v>
       </c>
-      <c r="E47" s="37" t="s">
+      <c r="E47" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="F47" s="37" t="s">
+      <c r="F47" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
       <c r="I47" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="35" t="s">
+      <c r="A48" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="B48" s="35" t="s">
+      <c r="B48" s="30" t="s">
         <v>156</v>
       </c>
-      <c r="C48" s="35" t="s">
+      <c r="C48" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="D48" s="39" t="n">
+      <c r="D48" s="34" t="n">
         <v>3</v>
       </c>
-      <c r="E48" s="37" t="s">
+      <c r="E48" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="F48" s="37" t="s">
+      <c r="F48" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
       <c r="I48" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="35" t="s">
+      <c r="A49" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="B49" s="35" t="s">
+      <c r="B49" s="30" t="s">
         <v>156</v>
       </c>
-      <c r="C49" s="35" t="s">
+      <c r="C49" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="D49" s="39" t="n">
+      <c r="D49" s="34" t="n">
         <v>4</v>
       </c>
-      <c r="E49" s="37" t="s">
+      <c r="E49" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="F49" s="37" t="s">
+      <c r="F49" s="32" t="s">
         <v>158</v>
       </c>
-      <c r="G49" s="17"/>
-      <c r="H49" s="17"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
       <c r="I49" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="35" t="s">
+      <c r="A50" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="B50" s="35" t="s">
+      <c r="B50" s="30" t="s">
         <v>162</v>
       </c>
-      <c r="C50" s="35" t="s">
+      <c r="C50" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="D50" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="E50" s="37" t="s">
+      <c r="D50" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="E50" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="F50" s="37" t="s">
+      <c r="F50" s="32" t="s">
         <v>122</v>
       </c>
       <c r="I50" s="1" t="s">
@@ -2624,22 +2588,22 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="35" t="s">
+      <c r="A51" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="B51" s="35" t="s">
+      <c r="B51" s="30" t="s">
         <v>162</v>
       </c>
-      <c r="C51" s="35" t="s">
+      <c r="C51" s="30" t="s">
         <v>164</v>
       </c>
-      <c r="D51" s="39" t="n">
+      <c r="D51" s="34" t="n">
         <v>2</v>
       </c>
-      <c r="E51" s="37" t="s">
+      <c r="E51" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="F51" s="37" t="s">
+      <c r="F51" s="32" t="s">
         <v>101</v>
       </c>
       <c r="I51" s="1" t="s">
@@ -2647,22 +2611,22 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="35" t="s">
+      <c r="A52" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="B52" s="35" t="s">
+      <c r="B52" s="30" t="s">
         <v>166</v>
       </c>
-      <c r="C52" s="35" t="s">
+      <c r="C52" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="D52" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="E52" s="37" t="s">
+      <c r="D52" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="E52" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="F52" s="37" t="s">
+      <c r="F52" s="32" t="s">
         <v>167</v>
       </c>
       <c r="I52" s="1" t="s">
@@ -2670,22 +2634,22 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="35" t="s">
+      <c r="A53" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="B53" s="35" t="s">
+      <c r="B53" s="30" t="s">
         <v>169</v>
       </c>
-      <c r="C53" s="35" t="s">
+      <c r="C53" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="D53" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="E53" s="37" t="s">
+      <c r="D53" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="E53" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="F53" s="37" t="s">
+      <c r="F53" s="32" t="s">
         <v>152</v>
       </c>
       <c r="I53" s="1" t="s">
@@ -2693,22 +2657,22 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="35" t="s">
+      <c r="A54" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="B54" s="35" t="s">
+      <c r="B54" s="30" t="s">
         <v>169</v>
       </c>
-      <c r="C54" s="35" t="s">
+      <c r="C54" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="D54" s="39" t="n">
+      <c r="D54" s="34" t="n">
         <v>2</v>
       </c>
-      <c r="E54" s="37" t="s">
+      <c r="E54" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="F54" s="37" t="s">
+      <c r="F54" s="32" t="s">
         <v>152</v>
       </c>
       <c r="I54" s="1" t="s">
@@ -2716,40 +2680,40 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="22" t="s">
+      <c r="A55" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="B55" s="22" t="s">
+      <c r="B55" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="C55" s="22" t="s">
+      <c r="C55" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="D55" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="E55" s="22" t="s">
+      <c r="D55" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="E55" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="F55" s="22"/>
+      <c r="F55" s="17"/>
       <c r="I55" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="17" t="s">
+      <c r="A56" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="B56" s="17" t="s">
+      <c r="B56" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="C56" s="17" t="s">
+      <c r="C56" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="D56" s="40" t="n">
-        <v>1</v>
-      </c>
-      <c r="E56" s="22" t="s">
+      <c r="D56" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="E56" s="17" t="s">
         <v>85</v>
       </c>
       <c r="I56" s="1" t="s">
@@ -2757,19 +2721,19 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="17" t="s">
+      <c r="A57" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="B57" s="17" t="s">
+      <c r="B57" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="C57" s="41" t="s">
-        <v>179</v>
-      </c>
-      <c r="D57" s="40" t="n">
-        <v>1</v>
-      </c>
-      <c r="E57" s="22" t="s">
+      <c r="C57" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="D57" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="E57" s="17" t="s">
         <v>85</v>
       </c>
       <c r="I57" s="1" t="s">
@@ -2777,19 +2741,19 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="17" t="s">
+      <c r="A58" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="B58" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="B58" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="C58" s="41" t="s">
-        <v>179</v>
-      </c>
-      <c r="D58" s="40" t="n">
-        <v>1</v>
-      </c>
-      <c r="E58" s="22" t="s">
+      <c r="C58" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="D58" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="E58" s="17" t="s">
         <v>85</v>
       </c>
       <c r="I58" s="1" t="s">
@@ -2797,19 +2761,19 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="17" t="s">
+      <c r="A59" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="B59" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="B59" s="17" t="s">
+      <c r="C59" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="C59" s="41" t="s">
-        <v>184</v>
-      </c>
-      <c r="D59" s="40" t="n">
-        <v>1</v>
-      </c>
-      <c r="E59" s="22" t="s">
+      <c r="D59" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="E59" s="17" t="s">
         <v>85</v>
       </c>
       <c r="I59" s="1" t="s">
@@ -2817,19 +2781,19 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="17" t="s">
+      <c r="A60" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="B60" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="B60" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="C60" s="41" t="s">
-        <v>184</v>
-      </c>
-      <c r="D60" s="40" t="n">
-        <v>1</v>
-      </c>
-      <c r="E60" s="22" t="s">
+      <c r="C60" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="D60" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="E60" s="17" t="s">
         <v>85</v>
       </c>
       <c r="I60" s="1" t="s">
@@ -2837,19 +2801,19 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="17" t="s">
+      <c r="A61" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="B61" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="B61" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="C61" s="17" t="s">
+      <c r="C61" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="D61" s="40" t="n">
-        <v>1</v>
-      </c>
-      <c r="E61" s="22" t="s">
+      <c r="D61" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="E61" s="17" t="s">
         <v>85</v>
       </c>
       <c r="I61" s="1" t="s">
@@ -2857,19 +2821,19 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="17" t="s">
+      <c r="A62" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="B62" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="B62" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="C62" s="17" t="s">
+      <c r="C62" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="D62" s="40" t="n">
-        <v>1</v>
-      </c>
-      <c r="E62" s="22" t="s">
+      <c r="D62" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="E62" s="17" t="s">
         <v>85</v>
       </c>
       <c r="I62" s="1" t="s">
@@ -2878,228 +2842,276 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>193</v>
-      </c>
       <c r="D63" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E63" s="22" t="s">
+      <c r="E63" s="17" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>195</v>
-      </c>
       <c r="C64" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D64" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E64" s="22" t="s">
+      <c r="E64" s="17" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>197</v>
-      </c>
       <c r="C65" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D65" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E65" s="22" t="s">
+      <c r="E65" s="17" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>200</v>
-      </c>
       <c r="D66" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E66" s="22" t="s">
+      <c r="E66" s="17" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="C67" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D67" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E67" s="22" t="s">
+      <c r="E67" s="17" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>204</v>
-      </c>
       <c r="C68" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D68" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E68" s="22" t="s">
+      <c r="E68" s="17" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D69" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E69" s="22" t="s">
+      <c r="E69" s="17" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="C70" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D70" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E70" s="22" t="s">
+      <c r="E70" s="17" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="C71" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D71" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E71" s="22" t="s">
+      <c r="E71" s="17" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>211</v>
+        <v>178</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D72" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E72" s="22" t="s">
+      <c r="E72" s="17" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D73" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E73" s="22" t="s">
+      <c r="E73" s="17" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D74" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E74" s="22" t="s">
+      <c r="E74" s="17" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D75" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E75" s="17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B76" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D75" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E75" s="22" t="s">
+      <c r="C76" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D76" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E76" s="17" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D77" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E77" s="17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D78" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E78" s="17" t="s">
+        <v>85</v>
+      </c>
+    </row>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
nova branch para os campos
</commit_message>
<xml_diff>
--- a/Elenco SME_2025-2-ICMC_corrigido.xlsx
+++ b/Elenco SME_2025-2-ICMC_corrigido.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jo_bi\OneDrive\Área de Trabalho\Mestrado\formularios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jo_bi\OneDrive\Área de Trabalho\formularios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBBB8F8-BEEC-4D42-8D3D-10D726A7DBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6657B1BC-44CB-4503-8CBC-3C94DC7FD79F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -597,9 +597,6 @@
     <t>Produção</t>
   </si>
   <si>
-    <t>PRG-0027</t>
-  </si>
-  <si>
     <t xml:space="preserve">Uma jornada lúdica pela topologia geométrica	</t>
   </si>
   <si>
@@ -754,6 +751,9 @@
   </si>
   <si>
     <t>carga</t>
+  </si>
+  <si>
+    <t>PRG0027</t>
   </si>
 </sst>
 </file>
@@ -972,6 +972,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -981,7 +982,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1384,10 +1384,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:P74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1408,41 +1409,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
     </row>
     <row r="2" spans="1:16" ht="91.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
+      <c r="A2" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="33" t="s">
+      <c r="J2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
       <c r="N2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1491,13 +1492,13 @@
         <v>17</v>
       </c>
       <c r="O3" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:16" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>18</v>
       </c>
@@ -1526,11 +1527,11 @@
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
-      <c r="P4" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P4" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>18</v>
       </c>
@@ -1559,8 +1560,11 @@
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
-    </row>
-    <row r="6" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P5" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>27</v>
       </c>
@@ -1589,8 +1593,11 @@
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
-    </row>
-    <row r="7" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P6" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>27</v>
       </c>
@@ -1619,8 +1626,11 @@
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
-    </row>
-    <row r="8" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P7" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>33</v>
       </c>
@@ -1649,8 +1659,11 @@
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
-    </row>
-    <row r="9" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P8" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>33</v>
       </c>
@@ -1679,8 +1692,11 @@
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
-    </row>
-    <row r="10" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P9" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>39</v>
       </c>
@@ -1709,8 +1725,11 @@
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
-    </row>
-    <row r="11" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P10" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>44</v>
       </c>
@@ -1739,8 +1758,11 @@
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
-    </row>
-    <row r="12" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P11" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>48</v>
       </c>
@@ -1769,8 +1791,11 @@
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
-    </row>
-    <row r="13" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P12" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>50</v>
       </c>
@@ -1799,8 +1824,11 @@
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
-    </row>
-    <row r="14" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P13" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>54</v>
       </c>
@@ -1829,8 +1857,11 @@
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
-    </row>
-    <row r="15" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P14" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="48.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>58</v>
       </c>
@@ -1859,8 +1890,11 @@
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
-    </row>
-    <row r="16" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P15" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="48" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>63</v>
       </c>
@@ -1889,8 +1923,11 @@
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
-    </row>
-    <row r="17" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P16" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>66</v>
       </c>
@@ -1919,8 +1956,11 @@
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
-    </row>
-    <row r="18" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P17" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>69</v>
       </c>
@@ -1949,8 +1989,11 @@
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
-    </row>
-    <row r="19" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P18" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>71</v>
       </c>
@@ -1979,8 +2022,11 @@
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
       <c r="N19" s="8"/>
-    </row>
-    <row r="20" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P19" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>73</v>
       </c>
@@ -2009,8 +2055,11 @@
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
       <c r="N20" s="8"/>
-    </row>
-    <row r="21" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P20" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>77</v>
       </c>
@@ -2039,8 +2088,11 @@
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
       <c r="N21" s="8"/>
-    </row>
-    <row r="22" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P21" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>79</v>
       </c>
@@ -2069,8 +2121,11 @@
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
       <c r="N22" s="8"/>
-    </row>
-    <row r="23" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P22" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>81</v>
       </c>
@@ -2099,8 +2154,11 @@
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P23" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
         <v>83</v>
       </c>
@@ -2127,8 +2185,11 @@
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
-    </row>
-    <row r="25" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P24" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
         <v>87</v>
       </c>
@@ -2155,8 +2216,11 @@
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
       <c r="N25" s="8"/>
-    </row>
-    <row r="26" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P25" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="30.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
         <v>89</v>
       </c>
@@ -2183,8 +2247,11 @@
       <c r="L26" s="8"/>
       <c r="M26" s="8"/>
       <c r="N26" s="8"/>
-    </row>
-    <row r="27" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P26" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>92</v>
       </c>
@@ -2213,8 +2280,11 @@
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
       <c r="N27" s="8"/>
-    </row>
-    <row r="28" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P27" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>97</v>
       </c>
@@ -2243,8 +2313,11 @@
       <c r="L28" s="8"/>
       <c r="M28" s="8"/>
       <c r="N28" s="8"/>
-    </row>
-    <row r="29" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P28" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>102</v>
       </c>
@@ -2273,8 +2346,11 @@
       <c r="L29" s="8"/>
       <c r="M29" s="8"/>
       <c r="N29" s="8"/>
-    </row>
-    <row r="30" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P29" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>107</v>
       </c>
@@ -2301,8 +2377,11 @@
       <c r="L30" s="8"/>
       <c r="M30" s="8"/>
       <c r="N30" s="8"/>
-    </row>
-    <row r="31" spans="1:14" s="20" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P30" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" s="20" customFormat="1" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
         <v>111</v>
       </c>
@@ -2331,8 +2410,11 @@
       <c r="L31" s="10"/>
       <c r="M31" s="10"/>
       <c r="N31" s="10"/>
-    </row>
-    <row r="32" spans="1:14" s="20" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P31" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" s="20" customFormat="1" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>115</v>
       </c>
@@ -2361,8 +2443,11 @@
       <c r="L32" s="10"/>
       <c r="M32" s="10"/>
       <c r="N32" s="10"/>
-    </row>
-    <row r="33" spans="1:14" s="20" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P32" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" s="20" customFormat="1" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>119</v>
       </c>
@@ -2391,8 +2476,11 @@
       <c r="L33" s="10"/>
       <c r="M33" s="10"/>
       <c r="N33" s="10"/>
-    </row>
-    <row r="34" spans="1:14" s="20" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P33" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" s="20" customFormat="1" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>123</v>
       </c>
@@ -2421,8 +2509,11 @@
       <c r="L34" s="10"/>
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
-    </row>
-    <row r="35" spans="1:14" s="20" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P34" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" s="20" customFormat="1" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="21" t="s">
         <v>126</v>
       </c>
@@ -2451,8 +2542,11 @@
       <c r="L35" s="10"/>
       <c r="M35" s="10"/>
       <c r="N35" s="10"/>
-    </row>
-    <row r="36" spans="1:14" s="20" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P35" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" s="20" customFormat="1" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>128</v>
       </c>
@@ -2481,8 +2575,11 @@
       <c r="L36" s="10"/>
       <c r="M36" s="10"/>
       <c r="N36" s="10"/>
-    </row>
-    <row r="37" spans="1:14" s="23" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P36" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" s="23" customFormat="1" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
         <v>130</v>
       </c>
@@ -2509,8 +2606,11 @@
       <c r="L37" s="12"/>
       <c r="M37" s="12"/>
       <c r="N37" s="12"/>
-    </row>
-    <row r="38" spans="1:14" s="23" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P37" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" s="23" customFormat="1" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
         <v>132</v>
       </c>
@@ -2537,8 +2637,11 @@
       <c r="L38" s="12"/>
       <c r="M38" s="12"/>
       <c r="N38" s="12"/>
-    </row>
-    <row r="39" spans="1:14" s="23" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P38" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" s="23" customFormat="1" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
         <v>134</v>
       </c>
@@ -2565,8 +2668,11 @@
       <c r="L39" s="12"/>
       <c r="M39" s="12"/>
       <c r="N39" s="12"/>
-    </row>
-    <row r="40" spans="1:14" s="23" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P39" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" s="23" customFormat="1" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
         <v>136</v>
       </c>
@@ -2593,8 +2699,11 @@
       <c r="L40" s="12"/>
       <c r="M40" s="12"/>
       <c r="N40" s="12"/>
-    </row>
-    <row r="41" spans="1:14" s="23" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P40" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" s="23" customFormat="1" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
         <v>139</v>
       </c>
@@ -2621,8 +2730,11 @@
       <c r="L41" s="12"/>
       <c r="M41" s="12"/>
       <c r="N41" s="12"/>
-    </row>
-    <row r="42" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P41" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="24" t="s">
         <v>141</v>
       </c>
@@ -2651,8 +2763,11 @@
       <c r="L42" s="8"/>
       <c r="M42" s="8"/>
       <c r="N42" s="8"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P42" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="24" t="s">
         <v>141</v>
       </c>
@@ -2676,8 +2791,11 @@
       <c r="I43" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="P43" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="24" t="s">
         <v>149</v>
       </c>
@@ -2701,8 +2819,11 @@
       <c r="I44" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P44" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="24" t="s">
         <v>149</v>
       </c>
@@ -2726,8 +2847,11 @@
       <c r="I45" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P45" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="24" t="s">
         <v>155</v>
       </c>
@@ -2751,8 +2875,11 @@
       <c r="I46" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P46" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="24" t="s">
         <v>155</v>
       </c>
@@ -2776,8 +2903,11 @@
       <c r="I47" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P47" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="24" t="s">
         <v>155</v>
       </c>
@@ -2801,8 +2931,11 @@
       <c r="I48" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="P48" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="24" t="s">
         <v>155</v>
       </c>
@@ -2826,8 +2959,11 @@
       <c r="I49" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P49" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="24" t="s">
         <v>161</v>
       </c>
@@ -2849,8 +2985,11 @@
       <c r="I50" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P50" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="24" t="s">
         <v>161</v>
       </c>
@@ -2872,8 +3011,11 @@
       <c r="I51" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="P51" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="24" t="s">
         <v>165</v>
       </c>
@@ -2895,8 +3037,11 @@
       <c r="I52" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P52" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="24" t="s">
         <v>168</v>
       </c>
@@ -2918,8 +3063,11 @@
       <c r="I53" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P53" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="24" t="s">
         <v>168</v>
       </c>
@@ -2941,16 +3089,19 @@
       <c r="I54" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="P54" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="B55" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="B55" s="12" t="s">
+      <c r="C55" s="12" t="s">
         <v>172</v>
-      </c>
-      <c r="C55" s="12" t="s">
-        <v>173</v>
       </c>
       <c r="D55" s="22">
         <v>1</v>
@@ -2962,16 +3113,19 @@
       <c r="I55" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="P55" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B56" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="C56" s="8" t="s">
         <v>175</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>176</v>
       </c>
       <c r="D56" s="29">
         <v>1</v>
@@ -2982,16 +3136,19 @@
       <c r="I56" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="P56" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B57" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="C57" s="30" t="s">
         <v>178</v>
-      </c>
-      <c r="C57" s="30" t="s">
-        <v>179</v>
       </c>
       <c r="D57" s="29">
         <v>1</v>
@@ -3002,16 +3159,19 @@
       <c r="I57" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="P57" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B58" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="B58" s="8" t="s">
-        <v>181</v>
-      </c>
       <c r="C58" s="30" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D58" s="29">
         <v>1</v>
@@ -3022,16 +3182,19 @@
       <c r="I58" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="P58" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B59" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="C59" s="30" t="s">
         <v>183</v>
-      </c>
-      <c r="C59" s="30" t="s">
-        <v>184</v>
       </c>
       <c r="D59" s="29">
         <v>1</v>
@@ -3042,16 +3205,19 @@
       <c r="I59" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="P59" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B60" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="B60" s="8" t="s">
-        <v>186</v>
-      </c>
       <c r="C60" s="30" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D60" s="29">
         <v>1</v>
@@ -3062,16 +3228,19 @@
       <c r="I60" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="P60" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B61" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="B61" s="8" t="s">
-        <v>188</v>
-      </c>
       <c r="C61" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D61" s="29">
         <v>1</v>
@@ -3082,16 +3251,19 @@
       <c r="I61" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="P61" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B62" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="B62" s="8" t="s">
-        <v>190</v>
-      </c>
       <c r="C62" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D62" s="29">
         <v>1</v>
@@ -3102,16 +3274,19 @@
       <c r="I62" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="P62" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>191</v>
+      </c>
+      <c r="B63" t="s">
         <v>192</v>
       </c>
-      <c r="B63" t="s">
-        <v>193</v>
-      </c>
       <c r="C63" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D63" s="2">
         <v>1</v>
@@ -3119,16 +3294,19 @@
       <c r="E63" s="12" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="P63" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
+        <v>193</v>
+      </c>
+      <c r="B64" t="s">
         <v>194</v>
       </c>
-      <c r="B64" t="s">
-        <v>195</v>
-      </c>
       <c r="C64" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D64" s="2">
         <v>1</v>
@@ -3136,16 +3314,19 @@
       <c r="E64" s="12" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="P64" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
+        <v>195</v>
+      </c>
+      <c r="B65" t="s">
         <v>196</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
         <v>197</v>
-      </c>
-      <c r="C65" t="s">
-        <v>198</v>
       </c>
       <c r="D65" s="2">
         <v>1</v>
@@ -3153,16 +3334,19 @@
       <c r="E65" s="12" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="P65" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
+        <v>198</v>
+      </c>
+      <c r="B66" t="s">
         <v>199</v>
       </c>
-      <c r="B66" t="s">
-        <v>200</v>
-      </c>
       <c r="C66" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D66" s="2">
         <v>1</v>
@@ -3170,16 +3354,19 @@
       <c r="E66" s="12" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="P66" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>200</v>
+      </c>
+      <c r="B67" t="s">
         <v>201</v>
       </c>
-      <c r="B67" t="s">
-        <v>202</v>
-      </c>
       <c r="C67" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D67" s="2">
         <v>1</v>
@@ -3187,16 +3374,19 @@
       <c r="E67" s="12" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="P67" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B68" t="s">
         <v>49</v>
       </c>
       <c r="C68" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D68" s="2">
         <v>1</v>
@@ -3204,16 +3394,19 @@
       <c r="E68" s="12" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="P68" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
+        <v>203</v>
+      </c>
+      <c r="B69" t="s">
         <v>204</v>
       </c>
-      <c r="B69" t="s">
-        <v>205</v>
-      </c>
       <c r="C69" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D69" s="2">
         <v>1</v>
@@ -3221,16 +3414,19 @@
       <c r="E69" s="12" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="P69" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
+        <v>205</v>
+      </c>
+      <c r="B70" t="s">
         <v>206</v>
       </c>
-      <c r="B70" t="s">
-        <v>207</v>
-      </c>
       <c r="C70" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D70" s="2">
         <v>1</v>
@@ -3238,16 +3434,19 @@
       <c r="E70" s="12" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="P70" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
+        <v>207</v>
+      </c>
+      <c r="B71" t="s">
         <v>208</v>
       </c>
-      <c r="B71" t="s">
-        <v>209</v>
-      </c>
       <c r="C71" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D71" s="2">
         <v>1</v>
@@ -3255,16 +3454,19 @@
       <c r="E71" s="12" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="P71" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
+        <v>209</v>
+      </c>
+      <c r="B72" t="s">
         <v>210</v>
       </c>
-      <c r="B72" t="s">
-        <v>211</v>
-      </c>
       <c r="C72" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D72" s="2">
         <v>1</v>
@@ -3272,16 +3474,19 @@
       <c r="E72" s="12" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="P72" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>211</v>
+      </c>
+      <c r="B73" t="s">
         <v>212</v>
       </c>
-      <c r="B73" t="s">
-        <v>213</v>
-      </c>
       <c r="C73" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D73" s="2">
         <v>1</v>
@@ -3289,16 +3494,19 @@
       <c r="E73" s="12" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="P73" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>213</v>
+      </c>
+      <c r="B74" t="s">
         <v>214</v>
       </c>
-      <c r="B74" t="s">
-        <v>215</v>
-      </c>
       <c r="C74" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D74" s="2">
         <v>1</v>
@@ -3306,9 +3514,18 @@
       <c r="E74" s="12" t="s">
         <v>85</v>
       </c>
+      <c r="P74" s="31">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:O74" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A3:O74" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="PRG-0027"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="3">
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A2:G2"/>

</xml_diff>

<commit_message>
Remoção MA5002 e alteração no código PRG-0027 para PRG0027
</commit_message>
<xml_diff>
--- a/Elenco SME_2025-2-ICMC_corrigido.xlsx
+++ b/Elenco SME_2025-2-ICMC_corrigido.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jo_bi\OneDrive\Área de Trabalho\Mestrado\formularios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jo_bi\OneDrive\Área de Trabalho\formularios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBBB8F8-BEEC-4D42-8D3D-10D726A7DBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036BECC6-7F4C-482D-BB94-5280C361E6AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$3:$O$74</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$3:$N$74</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Planilha1!$A$1:$I$41</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Planilha1!$3:$3</definedName>
   </definedNames>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="216">
   <si>
     <t>Elenco de disciplinas SME para 2025-2</t>
   </si>
@@ -597,9 +597,6 @@
     <t>Produção</t>
   </si>
   <si>
-    <t>PRG-0027</t>
-  </si>
-  <si>
     <t xml:space="preserve">Uma jornada lúdica pela topologia geométrica	</t>
   </si>
   <si>
@@ -750,10 +747,7 @@
     <t>Tópicos Avançados em Machine Learning</t>
   </si>
   <si>
-    <t>grupo</t>
-  </si>
-  <si>
-    <t>carga</t>
+    <t>PRG0027</t>
   </si>
 </sst>
 </file>
@@ -898,7 +892,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -981,7 +975,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1384,10 +1377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P74"/>
+  <dimension ref="A1:N74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1404,10 +1397,9 @@
     <col min="12" max="12" width="13.88671875" customWidth="1"/>
     <col min="13" max="13" width="19.88671875" customWidth="1"/>
     <col min="14" max="14" width="36" customWidth="1"/>
-    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
@@ -1425,7 +1417,7 @@
       <c r="M1" s="31"/>
       <c r="N1" s="31"/>
     </row>
-    <row r="2" spans="1:16" ht="91.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="91.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
@@ -1447,7 +1439,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1490,14 +1482,8 @@
       <c r="N3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>18</v>
       </c>
@@ -1526,11 +1512,8 @@
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
-      <c r="P4" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>18</v>
       </c>
@@ -1560,7 +1543,7 @@
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
     </row>
-    <row r="6" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>27</v>
       </c>
@@ -1590,7 +1573,7 @@
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
     </row>
-    <row r="7" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>27</v>
       </c>
@@ -1620,7 +1603,7 @@
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
     </row>
-    <row r="8" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>33</v>
       </c>
@@ -1650,7 +1633,7 @@
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
     </row>
-    <row r="9" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>33</v>
       </c>
@@ -1680,7 +1663,7 @@
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
     </row>
-    <row r="10" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>39</v>
       </c>
@@ -1710,7 +1693,7 @@
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
     </row>
-    <row r="11" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>44</v>
       </c>
@@ -1740,7 +1723,7 @@
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
     </row>
-    <row r="12" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>48</v>
       </c>
@@ -1770,7 +1753,7 @@
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
     </row>
-    <row r="13" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>50</v>
       </c>
@@ -1800,7 +1783,7 @@
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
     </row>
-    <row r="14" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>54</v>
       </c>
@@ -1830,7 +1813,7 @@
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
     </row>
-    <row r="15" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>58</v>
       </c>
@@ -1860,7 +1843,7 @@
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
     </row>
-    <row r="16" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>63</v>
       </c>
@@ -2944,13 +2927,13 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B55" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="B55" s="12" t="s">
+      <c r="C55" s="12" t="s">
         <v>172</v>
-      </c>
-      <c r="C55" s="12" t="s">
-        <v>173</v>
       </c>
       <c r="D55" s="22">
         <v>1</v>
@@ -2965,13 +2948,13 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B56" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="C56" s="8" t="s">
         <v>175</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>176</v>
       </c>
       <c r="D56" s="29">
         <v>1</v>
@@ -2985,13 +2968,13 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B57" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="C57" s="30" t="s">
         <v>178</v>
-      </c>
-      <c r="C57" s="30" t="s">
-        <v>179</v>
       </c>
       <c r="D57" s="29">
         <v>1</v>
@@ -3005,13 +2988,13 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B58" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="B58" s="8" t="s">
-        <v>181</v>
-      </c>
       <c r="C58" s="30" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D58" s="29">
         <v>1</v>
@@ -3025,13 +3008,13 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B59" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="C59" s="30" t="s">
         <v>183</v>
-      </c>
-      <c r="C59" s="30" t="s">
-        <v>184</v>
       </c>
       <c r="D59" s="29">
         <v>1</v>
@@ -3045,13 +3028,13 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B60" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="B60" s="8" t="s">
-        <v>186</v>
-      </c>
       <c r="C60" s="30" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D60" s="29">
         <v>1</v>
@@ -3065,13 +3048,13 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B61" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="B61" s="8" t="s">
-        <v>188</v>
-      </c>
       <c r="C61" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D61" s="29">
         <v>1</v>
@@ -3085,13 +3068,13 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B62" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="B62" s="8" t="s">
-        <v>190</v>
-      </c>
       <c r="C62" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D62" s="29">
         <v>1</v>
@@ -3105,13 +3088,13 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>191</v>
+      </c>
+      <c r="B63" t="s">
         <v>192</v>
       </c>
-      <c r="B63" t="s">
-        <v>193</v>
-      </c>
       <c r="C63" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D63" s="2">
         <v>1</v>
@@ -3122,13 +3105,13 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
+        <v>193</v>
+      </c>
+      <c r="B64" t="s">
         <v>194</v>
       </c>
-      <c r="B64" t="s">
-        <v>195</v>
-      </c>
       <c r="C64" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D64" s="2">
         <v>1</v>
@@ -3139,13 +3122,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
+        <v>195</v>
+      </c>
+      <c r="B65" t="s">
         <v>196</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
         <v>197</v>
-      </c>
-      <c r="C65" t="s">
-        <v>198</v>
       </c>
       <c r="D65" s="2">
         <v>1</v>
@@ -3156,13 +3139,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
+        <v>198</v>
+      </c>
+      <c r="B66" t="s">
         <v>199</v>
       </c>
-      <c r="B66" t="s">
-        <v>200</v>
-      </c>
       <c r="C66" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D66" s="2">
         <v>1</v>
@@ -3173,13 +3156,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>200</v>
+      </c>
+      <c r="B67" t="s">
         <v>201</v>
       </c>
-      <c r="B67" t="s">
-        <v>202</v>
-      </c>
       <c r="C67" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D67" s="2">
         <v>1</v>
@@ -3190,13 +3173,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B68" t="s">
         <v>49</v>
       </c>
       <c r="C68" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D68" s="2">
         <v>1</v>
@@ -3207,13 +3190,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
+        <v>203</v>
+      </c>
+      <c r="B69" t="s">
         <v>204</v>
       </c>
-      <c r="B69" t="s">
-        <v>205</v>
-      </c>
       <c r="C69" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D69" s="2">
         <v>1</v>
@@ -3224,13 +3207,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
+        <v>205</v>
+      </c>
+      <c r="B70" t="s">
         <v>206</v>
       </c>
-      <c r="B70" t="s">
-        <v>207</v>
-      </c>
       <c r="C70" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D70" s="2">
         <v>1</v>
@@ -3241,13 +3224,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
+        <v>207</v>
+      </c>
+      <c r="B71" t="s">
         <v>208</v>
       </c>
-      <c r="B71" t="s">
-        <v>209</v>
-      </c>
       <c r="C71" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D71" s="2">
         <v>1</v>
@@ -3258,13 +3241,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
+        <v>209</v>
+      </c>
+      <c r="B72" t="s">
         <v>210</v>
       </c>
-      <c r="B72" t="s">
-        <v>211</v>
-      </c>
       <c r="C72" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D72" s="2">
         <v>1</v>
@@ -3275,13 +3258,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>211</v>
+      </c>
+      <c r="B73" t="s">
         <v>212</v>
       </c>
-      <c r="B73" t="s">
-        <v>213</v>
-      </c>
       <c r="C73" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D73" s="2">
         <v>1</v>
@@ -3292,13 +3275,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>213</v>
+      </c>
+      <c r="B74" t="s">
         <v>214</v>
       </c>
-      <c r="B74" t="s">
-        <v>215</v>
-      </c>
       <c r="C74" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D74" s="2">
         <v>1</v>
@@ -3308,7 +3291,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:O74" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A3:N74" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="3">
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A2:G2"/>

</xml_diff>

<commit_message>
MAI5032 - Tópicos em Pesquisa Operacional
</commit_message>
<xml_diff>
--- a/Elenco SME_2025-2-ICMC_corrigido.xlsx
+++ b/Elenco SME_2025-2-ICMC_corrigido.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="224">
   <si>
     <t xml:space="preserve">Elenco de disciplinas SME para 2025-2</t>
   </si>
@@ -743,6 +743,12 @@
   </si>
   <si>
     <t xml:space="preserve">Tópicos Avançados em Machine Learning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAI5032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tópicos em Pesquisa Operacional</t>
   </si>
 </sst>
 </file>
@@ -1161,18 +1167,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ74"/>
+  <dimension ref="A1:AMJ75"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K37" activeCellId="0" sqref="K37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K76" activeCellId="0" sqref="K76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="19.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.89"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.12"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.67"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="8" min="7" style="0" width="20.45"/>
@@ -1186,7 +1192,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="36"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1207,7 +1213,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="91.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="65.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1232,7 +1238,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" s="9" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="9" customFormat="true" ht="42.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -1766,7 +1772,7 @@
       <c r="P15" s="11"/>
       <c r="Q15" s="11"/>
     </row>
-    <row r="16" customFormat="false" ht="29.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
         <v>69</v>
       </c>
@@ -1806,7 +1812,7 @@
       <c r="P16" s="11"/>
       <c r="Q16" s="11"/>
     </row>
-    <row r="17" customFormat="false" ht="29.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
         <v>72</v>
       </c>
@@ -2797,7 +2803,7 @@
       <c r="Q41" s="15"/>
       <c r="AMJ41" s="0"/>
     </row>
-    <row r="42" customFormat="false" ht="29.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="30.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="27" t="s">
         <v>148</v>
       </c>
@@ -2872,7 +2878,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="29.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="30.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="27" t="s">
         <v>156</v>
       </c>
@@ -3810,6 +3816,32 @@
       <c r="K74" s="11" t="n">
         <f aca="false">0.25*J74</f>
         <v>1</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="D75" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E75" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="I75" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="J75" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="K75" s="0" t="n">
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>